<commit_message>
Fillo-Awesome and Proud commit
</commit_message>
<xml_diff>
--- a/JavaSelWorks/src/main/resources/TryTwo.xlsx
+++ b/JavaSelWorks/src/main/resources/TryTwo.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
-    <t>Constraint</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>Eureka</t>
+  </si>
+  <si>
+    <t>YoN</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -387,34 +389,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>